<commit_message>
changes to gold standard, latex automatic formatting for report
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inès BLIN\PycharmProjects\cam_l95_intro_natural_language_syntax_parsing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E4C3DF-217F-408B-B6FF-141F3F069D54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF7FC28-38F0-42B0-9666-40713D4889B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" firstSheet="2" activeTab="8" xr2:uid="{5BFCFA74-47DA-4559-B24C-9E28D72A64D4}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" firstSheet="2" activeTab="7" xr2:uid="{5BFCFA74-47DA-4559-B24C-9E28D72A64D4}"/>
   </bookViews>
   <sheets>
     <sheet name="templ_hierarchy" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4970" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4970" uniqueCount="419">
   <si>
     <t>ok</t>
   </si>
@@ -995,9 +995,6 @@
     <t>17/3,</t>
   </si>
   <si>
-    <t>13/1,</t>
-  </si>
-  <si>
     <t>1/1,</t>
   </si>
   <si>
@@ -1061,12 +1058,6 @@
     <t>Instead</t>
   </si>
   <si>
-    <t>13/3,</t>
-  </si>
-  <si>
-    <t>21/8 ,</t>
-  </si>
-  <si>
     <t>23/2,</t>
   </si>
   <si>
@@ -1139,9 +1130,6 @@
     <t>0/1</t>
   </si>
   <si>
-    <t>3/1,</t>
-  </si>
-  <si>
     <t>nsubj:pass</t>
   </si>
   <si>
@@ -1163,9 +1151,6 @@
     <t>15/3,</t>
   </si>
   <si>
-    <t>9/1,</t>
-  </si>
-  <si>
     <t>13/0</t>
   </si>
   <si>
@@ -1181,9 +1166,6 @@
     <t>22/8,</t>
   </si>
   <si>
-    <t>24/4,</t>
-  </si>
-  <si>
     <t>22/3,</t>
   </si>
   <si>
@@ -1283,10 +1265,37 @@
     <t>10/4,</t>
   </si>
   <si>
-    <t>24/3,</t>
-  </si>
-  <si>
     <t>column=gold, line=parser</t>
+  </si>
+  <si>
+    <t>4/1,</t>
+  </si>
+  <si>
+    <t>15/1,</t>
+  </si>
+  <si>
+    <t>11/4,</t>
+  </si>
+  <si>
+    <t>24/2,</t>
+  </si>
+  <si>
+    <t>23/8,</t>
+  </si>
+  <si>
+    <t>25/4,</t>
+  </si>
+  <si>
+    <t>8/1,</t>
+  </si>
+  <si>
+    <t>25/3,</t>
+  </si>
+  <si>
+    <t>8/0</t>
+  </si>
+  <si>
+    <t>12/3,</t>
   </si>
 </sst>
 </file>
@@ -3573,7 +3582,7 @@
   <dimension ref="A1:AX50"/>
   <sheetViews>
     <sheetView zoomScale="38" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+      <selection activeCell="AJ37" sqref="AJ37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3631,7 +3640,7 @@
   <sheetData>
     <row r="1" spans="1:50" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3786,7 +3795,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="T2">
         <v>1</v>
@@ -3832,7 +3841,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -3844,11 +3853,9 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="13">
-        <v>1</v>
-      </c>
+      <c r="D5" s="13"/>
       <c r="E5" s="2" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -3870,7 +3877,7 @@
         <v>7</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
@@ -3930,7 +3937,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="K10" s="14"/>
       <c r="L10" s="8"/>
@@ -3974,7 +3981,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="18" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="M12" s="14"/>
       <c r="N12" s="14"/>
@@ -4000,7 +4007,7 @@
       <c r="K13" s="8"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="N13" s="14"/>
       <c r="O13" s="17"/>
@@ -4018,11 +4025,11 @@
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M14" s="14"/>
       <c r="N14" s="18" t="s">
-        <v>342</v>
+        <v>412</v>
       </c>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
@@ -4045,7 +4052,7 @@
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
       <c r="O15" s="8" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
@@ -4066,11 +4073,9 @@
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
-      <c r="O16" s="8">
-        <v>1</v>
-      </c>
+      <c r="O16" s="8"/>
       <c r="P16" s="14" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
@@ -4090,7 +4095,7 @@
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="R17" s="8"/>
     </row>
@@ -4110,7 +4115,7 @@
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="14" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
@@ -4171,7 +4176,7 @@
         <v>2</v>
       </c>
       <c r="T20" s="11" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
@@ -4202,7 +4207,7 @@
         <v>1</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
@@ -4302,7 +4307,7 @@
       <c r="V24" s="10"/>
       <c r="W24" s="19"/>
       <c r="X24" s="19" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="Y24" s="19"/>
       <c r="Z24" s="19"/>
@@ -4375,7 +4380,7 @@
       <c r="X26" s="19"/>
       <c r="Y26" s="19"/>
       <c r="Z26" s="19" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="AA26" s="19"/>
       <c r="AB26" s="19"/>
@@ -4443,7 +4448,7 @@
       <c r="Z28" s="19"/>
       <c r="AA28" s="19"/>
       <c r="AB28" s="19" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AC28" s="19"/>
       <c r="AD28" s="19"/>
@@ -4477,7 +4482,7 @@
       <c r="AA29" s="19"/>
       <c r="AB29" s="19"/>
       <c r="AC29" s="19" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AD29" s="19"/>
       <c r="AE29" s="19"/>
@@ -4511,7 +4516,7 @@
       <c r="AB30" s="19"/>
       <c r="AC30" s="19"/>
       <c r="AD30" s="23" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AE30" s="23"/>
       <c r="AF30" s="19"/>
@@ -4578,9 +4583,7 @@
       <c r="T32" s="10"/>
       <c r="U32" s="10"/>
       <c r="V32" s="10"/>
-      <c r="W32" s="19">
-        <v>1</v>
-      </c>
+      <c r="W32" s="19"/>
       <c r="X32" s="19"/>
       <c r="Y32" s="19"/>
       <c r="Z32" s="19"/>
@@ -4592,7 +4595,7 @@
         <v>1</v>
       </c>
       <c r="AF32" s="24" t="s">
-        <v>340</v>
+        <v>368</v>
       </c>
       <c r="AG32" s="23"/>
       <c r="AH32" s="19"/>
@@ -4656,9 +4659,7 @@
       <c r="V34" s="10"/>
       <c r="W34" s="19"/>
       <c r="X34" s="19"/>
-      <c r="Y34" s="19">
-        <v>1</v>
-      </c>
+      <c r="Y34" s="19"/>
       <c r="Z34" s="19"/>
       <c r="AA34" s="19"/>
       <c r="AB34" s="19"/>
@@ -4668,7 +4669,7 @@
       <c r="AF34" s="19"/>
       <c r="AG34" s="19"/>
       <c r="AH34" s="19" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="AI34" s="19"/>
       <c r="AJ34" s="19"/>
@@ -4702,7 +4703,7 @@
       <c r="AG35" s="19"/>
       <c r="AH35" s="19"/>
       <c r="AI35" s="21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AJ35" s="19"/>
       <c r="AK35" s="19"/>
@@ -4727,9 +4728,7 @@
       </c>
       <c r="U36" s="10"/>
       <c r="V36" s="10"/>
-      <c r="W36" s="19">
-        <v>1</v>
-      </c>
+      <c r="W36" s="19"/>
       <c r="X36" s="19"/>
       <c r="Y36" s="19"/>
       <c r="Z36" s="19"/>
@@ -4743,7 +4742,7 @@
       <c r="AH36" s="19"/>
       <c r="AI36" s="19"/>
       <c r="AJ36" s="21" t="s">
-        <v>318</v>
+        <v>371</v>
       </c>
       <c r="AK36" s="19"/>
       <c r="AL36" s="19"/>
@@ -4777,7 +4776,7 @@
       <c r="AI37" s="19"/>
       <c r="AJ37" s="19"/>
       <c r="AK37" s="23" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AL37" s="23"/>
       <c r="AM37" s="19"/>
@@ -4881,7 +4880,7 @@
       <c r="AL40" s="19"/>
       <c r="AM40" s="19"/>
       <c r="AN40" s="19" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AO40" s="20"/>
       <c r="AP40" s="20"/>
@@ -4902,9 +4901,7 @@
       <c r="Z41" s="19"/>
       <c r="AA41" s="19"/>
       <c r="AB41" s="19"/>
-      <c r="AC41" s="19">
-        <v>1</v>
-      </c>
+      <c r="AC41" s="19"/>
       <c r="AD41" s="19"/>
       <c r="AE41" s="19"/>
       <c r="AF41" s="19"/>
@@ -4917,7 +4914,7 @@
       <c r="AM41" s="19"/>
       <c r="AN41" s="19"/>
       <c r="AO41" s="22" t="s">
-        <v>341</v>
+        <v>374</v>
       </c>
       <c r="AP41" s="20"/>
       <c r="AQ41" s="20"/>
@@ -4953,7 +4950,7 @@
       <c r="AN42" s="19"/>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AQ42" s="20"/>
       <c r="AR42" s="20"/>
@@ -5046,7 +5043,7 @@
       <c r="AQ45" s="20"/>
       <c r="AR45" s="20"/>
       <c r="AS45" s="20" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="46" spans="1:48" x14ac:dyDescent="0.55000000000000004">
@@ -5062,7 +5059,7 @@
         <v>51</v>
       </c>
       <c r="AU47" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="48" spans="1:48" x14ac:dyDescent="0.55000000000000004">
@@ -5073,7 +5070,7 @@
         <v>1</v>
       </c>
       <c r="AV48" s="12" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="49" spans="1:50" x14ac:dyDescent="0.55000000000000004">
@@ -5081,7 +5078,7 @@
         <v>53</v>
       </c>
       <c r="AW49" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="50" spans="1:50" x14ac:dyDescent="0.55000000000000004">
@@ -5089,7 +5086,7 @@
         <v>55</v>
       </c>
       <c r="AX50" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -5104,7 +5101,7 @@
   <dimension ref="A1:AD166"/>
   <sheetViews>
     <sheetView zoomScale="34" workbookViewId="0">
-      <selection activeCell="V68" sqref="V68"/>
+      <selection activeCell="AB18" activeCellId="1" sqref="X18 AB18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5707,8 +5704,8 @@
       <c r="W9" s="3">
         <v>12</v>
       </c>
-      <c r="X9" s="6" t="s">
-        <v>18</v>
+      <c r="X9" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="Y9" s="3">
         <v>8</v>
@@ -5719,7 +5716,7 @@
       <c r="AA9">
         <v>12</v>
       </c>
-      <c r="AB9" s="6" t="s">
+      <c r="AB9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -5781,8 +5778,8 @@
       <c r="W10">
         <v>12</v>
       </c>
-      <c r="X10" s="6" t="s">
-        <v>3</v>
+      <c r="X10" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="Y10" s="3">
         <v>9</v>
@@ -5793,7 +5790,7 @@
       <c r="AA10">
         <v>12</v>
       </c>
-      <c r="AB10" s="6" t="s">
+      <c r="AB10" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5929,8 +5926,8 @@
       <c r="W12">
         <v>12</v>
       </c>
-      <c r="X12" s="6" t="s">
-        <v>27</v>
+      <c r="X12" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="Y12">
         <v>11</v>
@@ -5941,7 +5938,7 @@
       <c r="AA12">
         <v>12</v>
       </c>
-      <c r="AB12" s="6" t="s">
+      <c r="AB12" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -6373,8 +6370,8 @@
       <c r="W18" s="3">
         <v>18</v>
       </c>
-      <c r="X18" s="6" t="s">
-        <v>27</v>
+      <c r="X18" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="Y18" s="3">
         <v>17</v>
@@ -6385,7 +6382,7 @@
       <c r="AA18">
         <v>18</v>
       </c>
-      <c r="AB18" s="6" t="s">
+      <c r="AB18" s="13" t="s">
         <v>64</v>
       </c>
     </row>
@@ -6595,8 +6592,8 @@
       <c r="W21" s="3">
         <v>14</v>
       </c>
-      <c r="X21" s="6" t="s">
-        <v>29</v>
+      <c r="X21" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="Y21" s="3">
         <v>20</v>
@@ -6607,7 +6604,7 @@
       <c r="AA21">
         <v>14</v>
       </c>
-      <c r="AB21" s="6" t="s">
+      <c r="AB21" s="13" t="s">
         <v>78</v>
       </c>
     </row>
@@ -8248,11 +8245,11 @@
       <c r="B47" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C47" s="13">
         <v>5</v>
       </c>
-      <c r="D47" s="6" t="s">
-        <v>33</v>
+      <c r="D47" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="E47" s="3">
         <v>13</v>
@@ -8266,10 +8263,10 @@
       <c r="H47">
         <v>14</v>
       </c>
-      <c r="I47" s="6">
+      <c r="I47" s="13">
         <v>14</v>
       </c>
-      <c r="J47" s="6" t="s">
+      <c r="J47" s="13" t="s">
         <v>67</v>
       </c>
       <c r="L47" s="3">
@@ -8334,11 +8331,11 @@
       <c r="B48" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C48" s="6">
+      <c r="C48" s="13">
         <v>13</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>14</v>
+      <c r="D48" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="E48" s="3">
         <v>14</v>
@@ -8352,10 +8349,10 @@
       <c r="H48">
         <v>5</v>
       </c>
-      <c r="I48" s="6">
+      <c r="I48" s="13">
         <v>5</v>
       </c>
-      <c r="J48" s="6" t="s">
+      <c r="J48" s="13" t="s">
         <v>58</v>
       </c>
       <c r="L48" s="3">
@@ -13096,7 +13093,7 @@
         <v>1</v>
       </c>
       <c r="N129" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="O129" s="6">
         <v>2</v>
@@ -13108,7 +13105,7 @@
         <v>1</v>
       </c>
       <c r="R129" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="S129" s="6">
         <v>4</v>
@@ -13196,7 +13193,7 @@
         <v>3</v>
       </c>
       <c r="N131" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="O131" s="3">
         <v>4</v>
@@ -13208,7 +13205,7 @@
         <v>3</v>
       </c>
       <c r="R131" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="S131">
         <v>4</v>
@@ -13246,7 +13243,7 @@
         <v>4</v>
       </c>
       <c r="N132" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O132" s="6">
         <v>2</v>
@@ -13258,7 +13255,7 @@
         <v>4</v>
       </c>
       <c r="R132" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="S132" s="6">
         <v>13</v>
@@ -13346,7 +13343,7 @@
         <v>6</v>
       </c>
       <c r="N134" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O134" s="13">
         <v>5</v>
@@ -13358,7 +13355,7 @@
         <v>6</v>
       </c>
       <c r="R134" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="S134" s="13">
         <v>4</v>
@@ -13496,7 +13493,7 @@
         <v>9</v>
       </c>
       <c r="N137" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O137" s="3">
         <v>13</v>
@@ -13508,7 +13505,7 @@
         <v>9</v>
       </c>
       <c r="R137" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="S137">
         <v>13</v>
@@ -13596,7 +13593,7 @@
         <v>11</v>
       </c>
       <c r="N139" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="O139" s="3">
         <v>9</v>
@@ -13608,7 +13605,7 @@
         <v>11</v>
       </c>
       <c r="R139" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="S139">
         <v>9</v>
@@ -13646,7 +13643,7 @@
         <v>12</v>
       </c>
       <c r="N140" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O140" s="3">
         <v>13</v>
@@ -13658,7 +13655,7 @@
         <v>12</v>
       </c>
       <c r="R140" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="S140">
         <v>13</v>
@@ -13696,7 +13693,7 @@
         <v>13</v>
       </c>
       <c r="N141" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O141" s="3">
         <v>0</v>
@@ -13708,7 +13705,7 @@
         <v>13</v>
       </c>
       <c r="R141" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S141">
         <v>0</v>
@@ -13796,7 +13793,7 @@
         <v>15</v>
       </c>
       <c r="N143" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O143" s="3">
         <v>16</v>
@@ -13808,7 +13805,7 @@
         <v>15</v>
       </c>
       <c r="R143" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="S143">
         <v>16</v>
@@ -13846,7 +13843,7 @@
         <v>16</v>
       </c>
       <c r="N144" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="O144" s="13">
         <v>14</v>
@@ -13858,7 +13855,7 @@
         <v>16</v>
       </c>
       <c r="R144" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="S144" s="13">
         <v>13</v>
@@ -13998,7 +13995,7 @@
         <v>20</v>
       </c>
       <c r="N148" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="O148" s="13">
         <v>18</v>
@@ -14010,7 +14007,7 @@
         <v>20</v>
       </c>
       <c r="R148" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="S148" s="13">
         <v>13</v>
@@ -14050,7 +14047,7 @@
         <v>22</v>
       </c>
       <c r="N150" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="O150" s="3">
         <v>24</v>
@@ -14062,7 +14059,7 @@
         <v>22</v>
       </c>
       <c r="R150" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S150">
         <v>24</v>
@@ -14102,7 +14099,7 @@
         <v>24</v>
       </c>
       <c r="N152" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="O152" s="13">
         <v>21</v>
@@ -14114,7 +14111,7 @@
         <v>24</v>
       </c>
       <c r="R152" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="S152" s="13">
         <v>20</v>
@@ -14180,7 +14177,7 @@
         <v>27</v>
       </c>
       <c r="N155" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="O155" s="3">
         <v>28</v>
@@ -14192,7 +14189,7 @@
         <v>27</v>
       </c>
       <c r="R155" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="S155">
         <v>28</v>
@@ -14258,7 +14255,7 @@
         <v>30</v>
       </c>
       <c r="N158" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="O158" s="3">
         <v>28</v>
@@ -14270,7 +14267,7 @@
         <v>30</v>
       </c>
       <c r="R158" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="S158">
         <v>28</v>
@@ -14284,7 +14281,7 @@
         <v>31</v>
       </c>
       <c r="N159" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="O159" s="6">
         <v>30</v>
@@ -14296,7 +14293,7 @@
         <v>31</v>
       </c>
       <c r="R159" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="S159" s="6">
         <v>33</v>
@@ -14336,7 +14333,7 @@
         <v>33</v>
       </c>
       <c r="N161" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="O161" s="3">
         <v>30</v>
@@ -14348,7 +14345,7 @@
         <v>33</v>
       </c>
       <c r="R161" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="S161">
         <v>30</v>
@@ -14388,7 +14385,7 @@
         <v>35</v>
       </c>
       <c r="N163" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="O163" s="3">
         <v>33</v>
@@ -14400,7 +14397,7 @@
         <v>35</v>
       </c>
       <c r="R163" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="S163">
         <v>33</v>
@@ -14414,7 +14411,7 @@
         <v>36</v>
       </c>
       <c r="N164" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O164" s="3">
         <v>37</v>
@@ -14426,7 +14423,7 @@
         <v>36</v>
       </c>
       <c r="R164" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="S164">
         <v>37</v>
@@ -14440,7 +14437,7 @@
         <v>37</v>
       </c>
       <c r="N165" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O165" s="3">
         <v>33</v>
@@ -14452,7 +14449,7 @@
         <v>37</v>
       </c>
       <c r="R165" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="S165">
         <v>33</v>
@@ -14514,7 +14511,7 @@
         <v>2014</v>
       </c>
       <c r="R1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -14528,7 +14525,7 @@
         <v>58</v>
       </c>
       <c r="L2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="M2" t="s">
         <v>34</v>
@@ -14537,7 +14534,7 @@
         <v>13</v>
       </c>
       <c r="S2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -14554,7 +14551,7 @@
         <v>16</v>
       </c>
       <c r="S3" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
@@ -14734,7 +14731,7 @@
         <v>110</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -15692,7 +15689,7 @@
   <dimension ref="A1:XFD50"/>
   <sheetViews>
     <sheetView zoomScale="40" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:F52"/>
+      <selection activeCell="AJ37" sqref="AJ37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -15750,7 +15747,7 @@
   <sheetData>
     <row r="1" spans="1:50" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -15905,7 +15902,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="AT2">
         <v>1</v>
@@ -15916,7 +15913,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.55000000000000004">
@@ -15924,7 +15921,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -15938,7 +15935,7 @@
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="2" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -15957,7 +15954,7 @@
         <v>7</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
@@ -15977,7 +15974,7 @@
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="14" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
@@ -16021,7 +16018,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="K10" s="14"/>
       <c r="L10" s="8"/>
@@ -16064,7 +16061,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="18" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="M12" s="14"/>
       <c r="N12" s="14"/>
@@ -16087,7 +16084,7 @@
       <c r="K13" s="8"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="N13" s="14"/>
       <c r="O13" s="17"/>
@@ -16106,12 +16103,10 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="14">
-        <v>1</v>
-      </c>
+      <c r="L14" s="14"/>
       <c r="M14" s="14"/>
       <c r="N14" s="18" t="s">
-        <v>380</v>
+        <v>414</v>
       </c>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
@@ -16134,7 +16129,7 @@
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
       <c r="O15" s="14" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="P15" s="14">
         <v>1</v>
@@ -16157,11 +16152,9 @@
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
-      <c r="O16" s="14">
-        <v>1</v>
-      </c>
+      <c r="O16" s="14"/>
       <c r="P16" s="14" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
@@ -16181,7 +16174,7 @@
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="14" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="R17" s="14"/>
     </row>
@@ -16201,7 +16194,7 @@
       <c r="P18" s="8"/>
       <c r="Q18" s="14"/>
       <c r="R18" s="14" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
@@ -16230,7 +16223,7 @@
         <v>22</v>
       </c>
       <c r="S19" s="11" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="T19" s="10"/>
       <c r="U19" s="10"/>
@@ -16262,7 +16255,7 @@
         <v>1</v>
       </c>
       <c r="T20" s="25" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
@@ -16295,7 +16288,7 @@
         <v>1</v>
       </c>
       <c r="U21" s="11" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
@@ -16355,7 +16348,7 @@
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
       <c r="W23" s="19" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="X23" s="19"/>
       <c r="Y23" s="19"/>
@@ -16434,7 +16427,7 @@
       <c r="W25" s="19"/>
       <c r="X25" s="19"/>
       <c r="Y25" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Z25" s="19"/>
       <c r="AA25" s="19"/>
@@ -16470,7 +16463,7 @@
       <c r="X26" s="19"/>
       <c r="Y26" s="19"/>
       <c r="Z26" s="19" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="AA26" s="19"/>
       <c r="AB26" s="19"/>
@@ -16494,7 +16487,7 @@
       <c r="AR26" s="20"/>
       <c r="AS26" s="20"/>
       <c r="XFD26" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="27" spans="1:48 16384:16384" x14ac:dyDescent="0.55000000000000004">
@@ -16543,7 +16536,7 @@
       <c r="Z28" s="19"/>
       <c r="AA28" s="19"/>
       <c r="AB28" s="19" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AC28" s="19"/>
       <c r="AD28" s="19"/>
@@ -16577,7 +16570,7 @@
       <c r="AA29" s="19"/>
       <c r="AB29" s="19"/>
       <c r="AC29" s="19" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AD29" s="19"/>
       <c r="AE29" s="19"/>
@@ -16614,7 +16607,7 @@
       <c r="AB30" s="19"/>
       <c r="AC30" s="19"/>
       <c r="AD30" s="23" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AE30" s="23"/>
       <c r="AF30" s="19"/>
@@ -16686,9 +16679,7 @@
       </c>
       <c r="U32" s="10"/>
       <c r="V32" s="10"/>
-      <c r="W32" s="19">
-        <v>1</v>
-      </c>
+      <c r="W32" s="19"/>
       <c r="X32" s="19"/>
       <c r="Y32" s="19"/>
       <c r="Z32" s="19"/>
@@ -16698,7 +16689,7 @@
       <c r="AD32" s="19"/>
       <c r="AE32" s="19"/>
       <c r="AF32" s="24" t="s">
-        <v>376</v>
+        <v>410</v>
       </c>
       <c r="AG32" s="23">
         <v>2</v>
@@ -16736,7 +16727,7 @@
       <c r="AE33" s="19"/>
       <c r="AF33" s="23"/>
       <c r="AG33" s="23" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AH33" s="19"/>
       <c r="AI33" s="19"/>
@@ -16766,9 +16757,7 @@
       <c r="V34" s="10"/>
       <c r="W34" s="19"/>
       <c r="X34" s="19"/>
-      <c r="Y34" s="19">
-        <v>1</v>
-      </c>
+      <c r="Y34" s="19"/>
       <c r="Z34" s="19"/>
       <c r="AA34" s="19"/>
       <c r="AB34" s="19"/>
@@ -16778,7 +16767,7 @@
       <c r="AF34" s="19"/>
       <c r="AG34" s="19"/>
       <c r="AH34" s="19" t="s">
-        <v>366</v>
+        <v>409</v>
       </c>
       <c r="AI34" s="19"/>
       <c r="AJ34" s="19"/>
@@ -16815,7 +16804,7 @@
       <c r="AG35" s="19"/>
       <c r="AH35" s="19"/>
       <c r="AI35" s="21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AJ35" s="19"/>
       <c r="AK35" s="19"/>
@@ -16841,7 +16830,7 @@
       <c r="U36" s="10"/>
       <c r="V36" s="10"/>
       <c r="W36" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X36" s="19"/>
       <c r="Y36" s="19"/>
@@ -16856,7 +16845,7 @@
       <c r="AH36" s="19"/>
       <c r="AI36" s="19"/>
       <c r="AJ36" s="21" t="s">
-        <v>376</v>
+        <v>410</v>
       </c>
       <c r="AK36" s="19"/>
       <c r="AL36" s="19"/>
@@ -16890,7 +16879,7 @@
       <c r="AI37" s="19"/>
       <c r="AJ37" s="19"/>
       <c r="AK37" s="23" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AL37" s="23"/>
       <c r="AM37" s="19"/>
@@ -16994,7 +16983,7 @@
       <c r="AL40" s="19"/>
       <c r="AM40" s="19"/>
       <c r="AN40" s="19" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AO40" s="20"/>
       <c r="AP40" s="20"/>
@@ -17015,9 +17004,7 @@
       <c r="Z41" s="19"/>
       <c r="AA41" s="19"/>
       <c r="AB41" s="19"/>
-      <c r="AC41" s="19">
-        <v>1</v>
-      </c>
+      <c r="AC41" s="19"/>
       <c r="AD41" s="19"/>
       <c r="AE41" s="19"/>
       <c r="AF41" s="19">
@@ -17032,7 +17019,7 @@
       <c r="AM41" s="19"/>
       <c r="AN41" s="19"/>
       <c r="AO41" s="22" t="s">
-        <v>379</v>
+        <v>413</v>
       </c>
       <c r="AP41" s="20"/>
       <c r="AQ41" s="20"/>
@@ -17068,7 +17055,7 @@
       <c r="AN42" s="19"/>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AQ42" s="20"/>
       <c r="AR42" s="20"/>
@@ -17161,7 +17148,7 @@
       <c r="AQ45" s="20"/>
       <c r="AR45" s="20"/>
       <c r="AS45" s="20" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="46" spans="1:48" x14ac:dyDescent="0.55000000000000004">
@@ -17175,7 +17162,7 @@
         <v>1</v>
       </c>
       <c r="AT46" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47" spans="1:48" x14ac:dyDescent="0.55000000000000004">
@@ -17183,7 +17170,7 @@
         <v>51</v>
       </c>
       <c r="AU47" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="48" spans="1:48" x14ac:dyDescent="0.55000000000000004">
@@ -17194,7 +17181,7 @@
         <v>1</v>
       </c>
       <c r="AV48" s="12" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
     </row>
     <row r="49" spans="1:50" x14ac:dyDescent="0.55000000000000004">
@@ -17202,7 +17189,7 @@
         <v>53</v>
       </c>
       <c r="AW49" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="50" spans="1:50" x14ac:dyDescent="0.55000000000000004">
@@ -17210,7 +17197,7 @@
         <v>55</v>
       </c>
       <c r="AX50" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -17222,8 +17209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659D9681-9BEB-4DFB-B3D6-E017511B59AC}">
   <dimension ref="A1:AI114"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="49" workbookViewId="0">
-      <selection activeCell="AF24" sqref="AF24"/>
+    <sheetView topLeftCell="A30" zoomScale="49" workbookViewId="0">
+      <selection activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -17233,25 +17220,25 @@
         <v>110</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>110</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="S1" s="9" t="s">
         <v>110</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="AB1" s="9" t="s">
         <v>110</v>
       </c>
       <c r="AF1" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -17455,7 +17442,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -17467,7 +17454,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -17553,7 +17540,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -17565,7 +17552,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G5">
         <v>6</v>
@@ -17749,7 +17736,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -17761,7 +17748,7 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -18043,7 +18030,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C10">
         <v>6</v>
@@ -18055,7 +18042,7 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G10">
         <v>6</v>
@@ -18141,7 +18128,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C11" s="13">
         <v>9</v>
@@ -18153,7 +18140,7 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G11" s="13">
         <v>11</v>
@@ -18239,7 +18226,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C12" s="13">
         <v>10</v>
@@ -18251,13 +18238,13 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G12" s="13">
         <v>9</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="J12" s="3">
         <v>11</v>
@@ -18337,7 +18324,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C13">
         <v>13</v>
@@ -18349,7 +18336,7 @@
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G13" s="13">
         <v>13</v>
@@ -18435,7 +18422,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C14">
         <v>9</v>
@@ -18447,13 +18434,13 @@
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G14">
         <v>9</v>
       </c>
       <c r="H14" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="J14" s="3">
         <v>13</v>
@@ -18461,11 +18448,11 @@
       <c r="K14" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="13">
         <v>5</v>
       </c>
-      <c r="M14" s="6" t="s">
-        <v>33</v>
+      <c r="M14" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="N14" s="3">
         <v>13</v>
@@ -18473,10 +18460,10 @@
       <c r="O14" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="P14" s="6">
+      <c r="P14" s="13">
         <v>14</v>
       </c>
-      <c r="Q14" s="6" t="s">
+      <c r="Q14" s="13" t="s">
         <v>67</v>
       </c>
       <c r="S14" s="3">
@@ -18533,7 +18520,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C15" s="13">
         <v>9</v>
@@ -18545,7 +18532,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G15" s="13">
         <v>15</v>
@@ -18559,11 +18546,11 @@
       <c r="K15" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="13">
         <v>13</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>14</v>
+      <c r="M15" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="N15" s="3">
         <v>14</v>
@@ -18571,10 +18558,10 @@
       <c r="O15" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="P15" s="6">
+      <c r="P15" s="13">
         <v>5</v>
       </c>
-      <c r="Q15" s="6" t="s">
+      <c r="Q15" s="13" t="s">
         <v>58</v>
       </c>
       <c r="S15" s="3">
@@ -18599,7 +18586,7 @@
         <v>12</v>
       </c>
       <c r="Z15" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="AB15" s="3">
         <v>14</v>
@@ -18631,7 +18618,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C16" s="13">
         <v>14</v>
@@ -18643,13 +18630,13 @@
         <v>15</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G16" s="13">
         <v>9</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="J16" s="3">
         <v>15</v>
@@ -18721,7 +18708,7 @@
         <v>13</v>
       </c>
       <c r="AI16" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -18869,7 +18856,7 @@
         <v>12</v>
       </c>
       <c r="Z18" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="AB18" s="3">
         <v>17</v>
@@ -18901,7 +18888,7 @@
         <v>110</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="J19" s="3">
         <v>18</v>
@@ -20763,7 +20750,7 @@
         <v>16</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="J38" s="3">
         <v>37</v>
@@ -20909,7 +20896,7 @@
         <v>35</v>
       </c>
       <c r="Z39" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="AB39" s="3">
         <v>38</v>
@@ -21161,7 +21148,7 @@
         <v>110</v>
       </c>
       <c r="W42" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="AB42" s="3">
         <v>41</v>
@@ -21211,7 +21198,7 @@
         <v>16</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="J43" s="3">
         <v>42</v>
@@ -21339,7 +21326,7 @@
         <v>110</v>
       </c>
       <c r="AF44" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -21395,7 +21382,7 @@
         <v>1</v>
       </c>
       <c r="AC45" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AD45" s="6">
         <v>2</v>
@@ -21407,7 +21394,7 @@
         <v>1</v>
       </c>
       <c r="AG45" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AH45" s="6">
         <v>4</v>
@@ -21421,7 +21408,7 @@
         <v>110</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="J46" s="3">
         <v>45</v>
@@ -21573,7 +21560,7 @@
         <v>3</v>
       </c>
       <c r="AC47" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AD47" s="3">
         <v>4</v>
@@ -21585,7 +21572,7 @@
         <v>3</v>
       </c>
       <c r="AG47" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AH47">
         <v>4</v>
@@ -21671,7 +21658,7 @@
         <v>4</v>
       </c>
       <c r="AC48" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AD48" s="6">
         <v>2</v>
@@ -21683,7 +21670,7 @@
         <v>4</v>
       </c>
       <c r="AG48" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AH48" s="6">
         <v>13</v>
@@ -21848,8 +21835,8 @@
       <c r="U50" s="3">
         <v>12</v>
       </c>
-      <c r="V50" s="6" t="s">
-        <v>18</v>
+      <c r="V50" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="W50" s="3">
         <v>8</v>
@@ -21860,14 +21847,14 @@
       <c r="Y50">
         <v>12</v>
       </c>
-      <c r="Z50" s="6" t="s">
-        <v>367</v>
+      <c r="Z50" s="3" t="s">
+        <v>363</v>
       </c>
       <c r="AB50" s="3">
         <v>6</v>
       </c>
       <c r="AC50" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AD50" s="13">
         <v>5</v>
@@ -21879,13 +21866,13 @@
         <v>6</v>
       </c>
       <c r="AG50" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AH50" s="13">
         <v>4</v>
       </c>
       <c r="AI50" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -21946,8 +21933,8 @@
       <c r="U51">
         <v>12</v>
       </c>
-      <c r="V51" s="6" t="s">
-        <v>3</v>
+      <c r="V51" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="W51" s="3">
         <v>9</v>
@@ -21958,8 +21945,8 @@
       <c r="Y51">
         <v>12</v>
       </c>
-      <c r="Z51" s="6" t="s">
-        <v>368</v>
+      <c r="Z51" s="3" t="s">
+        <v>364</v>
       </c>
       <c r="AB51" s="3">
         <v>7</v>
@@ -22131,7 +22118,7 @@
         <v>45</v>
       </c>
       <c r="Q53" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="S53" s="3">
         <v>11</v>
@@ -22142,8 +22129,8 @@
       <c r="U53">
         <v>12</v>
       </c>
-      <c r="V53" s="6" t="s">
-        <v>27</v>
+      <c r="V53" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="W53" s="3">
         <v>11</v>
@@ -22154,14 +22141,14 @@
       <c r="Y53">
         <v>12</v>
       </c>
-      <c r="Z53" s="6" t="s">
+      <c r="Z53" s="3" t="s">
         <v>36</v>
       </c>
       <c r="AB53" s="3">
         <v>9</v>
       </c>
       <c r="AC53" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AD53" s="3">
         <v>13</v>
@@ -22173,7 +22160,7 @@
         <v>9</v>
       </c>
       <c r="AG53" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AH53">
         <v>13</v>
@@ -22333,7 +22320,7 @@
         <v>11</v>
       </c>
       <c r="AC55" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AD55" s="3">
         <v>9</v>
@@ -22345,7 +22332,7 @@
         <v>11</v>
       </c>
       <c r="AG55" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AH55">
         <v>9</v>
@@ -22383,7 +22370,7 @@
         <v>110</v>
       </c>
       <c r="N56" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="S56" s="3">
         <v>14</v>
@@ -22407,13 +22394,13 @@
         <v>12</v>
       </c>
       <c r="Z56" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="AB56" s="3">
         <v>12</v>
       </c>
       <c r="AC56" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AD56" s="3">
         <v>13</v>
@@ -22425,7 +22412,7 @@
         <v>12</v>
       </c>
       <c r="AG56" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AH56">
         <v>13</v>
@@ -22511,7 +22498,7 @@
         <v>13</v>
       </c>
       <c r="AC57" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AD57" s="3">
         <v>0</v>
@@ -22523,7 +22510,7 @@
         <v>13</v>
       </c>
       <c r="AG57" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AH57">
         <v>0</v>
@@ -22688,8 +22675,8 @@
       <c r="U59" s="3">
         <v>18</v>
       </c>
-      <c r="V59" s="6" t="s">
-        <v>27</v>
+      <c r="V59" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="W59" s="3">
         <v>17</v>
@@ -22700,14 +22687,14 @@
       <c r="Y59">
         <v>18</v>
       </c>
-      <c r="Z59" s="6" t="s">
+      <c r="Z59" s="13" t="s">
         <v>64</v>
       </c>
       <c r="AB59" s="3">
         <v>15</v>
       </c>
       <c r="AC59" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AD59" s="3">
         <v>16</v>
@@ -22719,7 +22706,7 @@
         <v>15</v>
       </c>
       <c r="AG59" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AH59">
         <v>16</v>
@@ -22775,7 +22762,7 @@
         <v>6</v>
       </c>
       <c r="Q60" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="S60" s="3">
         <v>18</v>
@@ -22805,7 +22792,7 @@
         <v>16</v>
       </c>
       <c r="AC60" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AD60" s="13">
         <v>14</v>
@@ -22817,13 +22804,13 @@
         <v>16</v>
       </c>
       <c r="AG60" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AH60" s="13">
         <v>13</v>
       </c>
       <c r="AI60" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -22873,7 +22860,7 @@
         <v>6</v>
       </c>
       <c r="Q61" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="S61" s="3">
         <v>19</v>
@@ -22982,8 +22969,8 @@
       <c r="U62" s="3">
         <v>14</v>
       </c>
-      <c r="V62" s="6" t="s">
-        <v>29</v>
+      <c r="V62" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="W62" s="3">
         <v>20</v>
@@ -22994,7 +22981,7 @@
       <c r="Y62">
         <v>14</v>
       </c>
-      <c r="Z62" s="6" t="s">
+      <c r="Z62" s="13" t="s">
         <v>78</v>
       </c>
       <c r="AB62" s="3">
@@ -23197,7 +23184,7 @@
         <v>20</v>
       </c>
       <c r="AC64" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AD64" s="13">
         <v>18</v>
@@ -23209,13 +23196,13 @@
         <v>20</v>
       </c>
       <c r="AG64" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AH64" s="13">
         <v>13</v>
       </c>
       <c r="AI64" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -23289,7 +23276,7 @@
         <v>20</v>
       </c>
       <c r="Z65" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="AB65" s="3">
         <v>21</v>
@@ -23393,7 +23380,7 @@
         <v>22</v>
       </c>
       <c r="AC66" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AD66" s="3">
         <v>24</v>
@@ -23405,7 +23392,7 @@
         <v>22</v>
       </c>
       <c r="AG66" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AH66">
         <v>24</v>
@@ -23461,7 +23448,7 @@
         <v>6</v>
       </c>
       <c r="Q67" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="S67" s="3">
         <v>25</v>
@@ -23589,7 +23576,7 @@
         <v>24</v>
       </c>
       <c r="AC68" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AD68" s="13">
         <v>21</v>
@@ -23601,7 +23588,7 @@
         <v>24</v>
       </c>
       <c r="AG68" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AH68" s="13">
         <v>20</v>
@@ -23853,7 +23840,7 @@
         <v>14</v>
       </c>
       <c r="Q71" s="6" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="S71" s="3">
         <v>29</v>
@@ -23877,13 +23864,13 @@
         <v>34</v>
       </c>
       <c r="Z71" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="AB71" s="3">
         <v>27</v>
       </c>
       <c r="AC71" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AD71" s="3">
         <v>28</v>
@@ -23895,7 +23882,7 @@
         <v>27</v>
       </c>
       <c r="AG71" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AH71">
         <v>28</v>
@@ -24073,7 +24060,7 @@
         <v>34</v>
       </c>
       <c r="Z73" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="AB73" s="3">
         <v>29</v>
@@ -24147,7 +24134,7 @@
         <v>9</v>
       </c>
       <c r="Q74" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="S74" s="3">
         <v>32</v>
@@ -24171,13 +24158,13 @@
         <v>34</v>
       </c>
       <c r="Z74" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="AB74" s="3">
         <v>30</v>
       </c>
       <c r="AC74" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AD74" s="3">
         <v>28</v>
@@ -24189,7 +24176,7 @@
         <v>30</v>
       </c>
       <c r="AG74" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AH74">
         <v>28</v>
@@ -24275,7 +24262,7 @@
         <v>31</v>
       </c>
       <c r="AC75" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AD75" s="3">
         <v>30</v>
@@ -24287,7 +24274,7 @@
         <v>31</v>
       </c>
       <c r="AG75" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AH75">
         <v>30</v>
@@ -24447,7 +24434,7 @@
         <v>33</v>
       </c>
       <c r="AC77" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AD77" s="3">
         <v>30</v>
@@ -24459,7 +24446,7 @@
         <v>33</v>
       </c>
       <c r="AG77" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AH77">
         <v>30</v>
@@ -24547,13 +24534,13 @@
         <v>110</v>
       </c>
       <c r="W79" s="9" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="AB79" s="3">
         <v>35</v>
       </c>
       <c r="AC79" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AD79" s="3">
         <v>33</v>
@@ -24565,7 +24552,7 @@
         <v>35</v>
       </c>
       <c r="AG79" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AH79">
         <v>33</v>
@@ -24627,7 +24614,7 @@
         <v>36</v>
       </c>
       <c r="AC80" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AD80" s="3">
         <v>37</v>
@@ -24639,7 +24626,7 @@
         <v>36</v>
       </c>
       <c r="AG80" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AH80">
         <v>37</v>
@@ -24701,7 +24688,7 @@
         <v>37</v>
       </c>
       <c r="AC81" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AD81" s="6">
         <v>33</v>
@@ -24713,7 +24700,7 @@
         <v>37</v>
       </c>
       <c r="AG81" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AH81" s="6">
         <v>35</v>
@@ -24993,7 +24980,7 @@
         <v>13</v>
       </c>
       <c r="Z86" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="87" spans="10:35" x14ac:dyDescent="0.55000000000000004">
@@ -25243,7 +25230,7 @@
         <v>13</v>
       </c>
       <c r="Z91" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="92" spans="10:35" x14ac:dyDescent="0.55000000000000004">
@@ -25593,7 +25580,7 @@
         <v>17</v>
       </c>
       <c r="Z98" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="99" spans="10:26" x14ac:dyDescent="0.55000000000000004">
@@ -25793,7 +25780,7 @@
         <v>17</v>
       </c>
       <c r="Z102" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="103" spans="10:26" x14ac:dyDescent="0.55000000000000004">
@@ -25893,7 +25880,7 @@
         <v>28</v>
       </c>
       <c r="Z104" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="105" spans="10:26" x14ac:dyDescent="0.55000000000000004">
@@ -25993,7 +25980,7 @@
         <v>28</v>
       </c>
       <c r="Z106" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="107" spans="10:26" x14ac:dyDescent="0.55000000000000004">
@@ -26143,7 +26130,7 @@
         <v>28</v>
       </c>
       <c r="Z109" s="13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="110" spans="10:26" x14ac:dyDescent="0.55000000000000004">
@@ -26357,8 +26344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838DEDFD-B7FA-4B94-B3CC-959D26B5945A}">
   <dimension ref="A1:XFD50"/>
   <sheetViews>
-    <sheetView zoomScale="36" workbookViewId="0">
-      <selection activeCell="AJ62" sqref="AJ62"/>
+    <sheetView tabSelected="1" zoomScale="36" workbookViewId="0">
+      <selection activeCell="AJ37" sqref="AJ37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -26416,7 +26403,7 @@
   <sheetData>
     <row r="1" spans="1:50" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -26582,7 +26569,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.55000000000000004">
@@ -26590,7 +26577,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>236</v>
+        <v>417</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -26604,7 +26591,7 @@
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="2" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -26623,7 +26610,7 @@
         <v>7</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
@@ -26669,7 +26656,7 @@
       <c r="G9" s="17"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
@@ -26697,7 +26684,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K10" s="14"/>
       <c r="L10" s="8"/>
@@ -26743,7 +26730,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
       <c r="L12" s="18" t="s">
-        <v>374</v>
+        <v>415</v>
       </c>
       <c r="M12" s="14"/>
       <c r="N12" s="14"/>
@@ -26811,7 +26798,7 @@
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
       <c r="N14" s="18" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
@@ -26833,7 +26820,7 @@
         <v>1</v>
       </c>
       <c r="O15" s="14" t="s">
-        <v>340</v>
+        <v>418</v>
       </c>
       <c r="P15" s="14"/>
       <c r="Q15" s="8"/>
@@ -26862,7 +26849,7 @@
       <c r="N16" s="17"/>
       <c r="O16" s="14"/>
       <c r="P16" s="14" t="s">
-        <v>261</v>
+        <v>235</v>
       </c>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
@@ -26885,7 +26872,7 @@
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="14" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="R17" s="14"/>
       <c r="Y17">
@@ -26908,7 +26895,7 @@
       <c r="P18" s="8"/>
       <c r="Q18" s="14"/>
       <c r="R18" s="14" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
@@ -26937,7 +26924,7 @@
         <v>22</v>
       </c>
       <c r="S19" s="11" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="T19" s="10"/>
       <c r="U19" s="10"/>
@@ -26978,7 +26965,7 @@
         <v>2</v>
       </c>
       <c r="T20" s="25" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
@@ -27014,7 +27001,7 @@
       </c>
       <c r="T21" s="10"/>
       <c r="U21" s="11" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
@@ -27074,7 +27061,7 @@
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
       <c r="W23" s="19" t="s">
-        <v>372</v>
+        <v>418</v>
       </c>
       <c r="X23" s="19"/>
       <c r="Y23" s="19"/>
@@ -27110,7 +27097,7 @@
       <c r="V24" s="10"/>
       <c r="W24" s="19"/>
       <c r="X24" s="19" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="Y24" s="19"/>
       <c r="Z24" s="19"/>
@@ -27147,7 +27134,7 @@
       <c r="W25" s="19"/>
       <c r="X25" s="19"/>
       <c r="Y25" s="19" t="s">
-        <v>173</v>
+        <v>345</v>
       </c>
       <c r="Z25" s="19"/>
       <c r="AA25" s="19"/>
@@ -27189,7 +27176,7 @@
       <c r="X26" s="19"/>
       <c r="Y26" s="19"/>
       <c r="Z26" s="19" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="AA26" s="19"/>
       <c r="AB26" s="19"/>
@@ -27211,7 +27198,7 @@
       <c r="AR26" s="20"/>
       <c r="AS26" s="20"/>
       <c r="XFD26" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="27" spans="1:46 16384:16384" x14ac:dyDescent="0.55000000000000004">
@@ -27226,7 +27213,7 @@
       <c r="Y27" s="19"/>
       <c r="Z27" s="19"/>
       <c r="AA27" s="19" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="AB27" s="19"/>
       <c r="AC27" s="19"/>
@@ -27260,7 +27247,7 @@
       <c r="Z28" s="19"/>
       <c r="AA28" s="19"/>
       <c r="AB28" s="19" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AC28" s="19"/>
       <c r="AD28" s="19"/>
@@ -27294,7 +27281,7 @@
       <c r="AA29" s="19"/>
       <c r="AB29" s="19"/>
       <c r="AC29" s="19" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AD29" s="19"/>
       <c r="AE29" s="19"/>
@@ -27362,7 +27349,7 @@
       <c r="AC31" s="19"/>
       <c r="AD31" s="23"/>
       <c r="AE31" s="23" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="AF31" s="19"/>
       <c r="AG31" s="19"/>
@@ -27399,7 +27386,7 @@
       <c r="AD32" s="19"/>
       <c r="AE32" s="19"/>
       <c r="AF32" s="24" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AG32" s="23"/>
       <c r="AH32" s="19"/>
@@ -27470,7 +27457,7 @@
       <c r="AF34" s="19"/>
       <c r="AG34" s="19"/>
       <c r="AH34" s="19" t="s">
-        <v>173</v>
+        <v>261</v>
       </c>
       <c r="AI34" s="19"/>
       <c r="AJ34" s="19"/>
@@ -27504,7 +27491,7 @@
       <c r="AG35" s="19"/>
       <c r="AH35" s="19"/>
       <c r="AI35" s="21" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="AJ35" s="19"/>
       <c r="AK35" s="19"/>
@@ -27545,7 +27532,7 @@
       <c r="AH36" s="19"/>
       <c r="AI36" s="19"/>
       <c r="AJ36" s="21" t="s">
-        <v>318</v>
+        <v>371</v>
       </c>
       <c r="AK36" s="19"/>
       <c r="AL36" s="19"/>
@@ -27579,7 +27566,7 @@
       <c r="AI37" s="19"/>
       <c r="AJ37" s="19"/>
       <c r="AK37" s="23" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AL37" s="23"/>
       <c r="AM37" s="19"/>
@@ -27681,7 +27668,7 @@
       <c r="AL40" s="19"/>
       <c r="AM40" s="19"/>
       <c r="AN40" s="19" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AO40" s="20"/>
       <c r="AP40" s="20"/>
@@ -27715,7 +27702,7 @@
       <c r="AM41" s="19"/>
       <c r="AN41" s="19"/>
       <c r="AO41" s="22" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="AP41" s="20"/>
       <c r="AQ41" s="20"/>
@@ -27749,7 +27736,7 @@
       <c r="AN42" s="19"/>
       <c r="AO42" s="20"/>
       <c r="AP42" s="20" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AQ42" s="20"/>
       <c r="AR42" s="20"/>
@@ -27780,7 +27767,7 @@
       <c r="AO43" s="20"/>
       <c r="AP43" s="20"/>
       <c r="AQ43" s="20" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="AR43" s="20"/>
       <c r="AS43" s="20"/>
@@ -27858,14 +27845,14 @@
       <c r="W46">
         <v>1</v>
       </c>
-      <c r="AC46">
+      <c r="AO46">
         <v>1</v>
       </c>
       <c r="AP46">
         <v>1</v>
       </c>
       <c r="AT46" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47" spans="1:48" x14ac:dyDescent="0.55000000000000004">
@@ -27873,7 +27860,7 @@
         <v>51</v>
       </c>
       <c r="AU47" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="48" spans="1:48" x14ac:dyDescent="0.55000000000000004">
@@ -27881,7 +27868,7 @@
         <v>52</v>
       </c>
       <c r="AV48" s="12" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="49" spans="1:50" x14ac:dyDescent="0.55000000000000004">
@@ -27889,7 +27876,7 @@
         <v>53</v>
       </c>
       <c r="AW49" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="50" spans="1:50" x14ac:dyDescent="0.55000000000000004">
@@ -27897,7 +27884,7 @@
         <v>55</v>
       </c>
       <c r="AX50" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -27909,8 +27896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A0DFB1-C4BA-4B13-85CC-8E889BF0DBB6}">
   <dimension ref="A1:Z179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L9" zoomScale="57" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+    <sheetView zoomScale="57" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -27930,7 +27917,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="28" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -27940,7 +27927,7 @@
       <c r="G2" s="28"/>
       <c r="H2" s="28"/>
       <c r="J2" s="28" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="K2" s="28"/>
       <c r="L2" s="28"/>
@@ -27950,7 +27937,7 @@
       <c r="P2" s="28"/>
       <c r="Q2" s="28"/>
       <c r="S2" s="28" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="T2" s="28"/>
       <c r="U2" s="28"/>
@@ -27968,7 +27955,7 @@
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
@@ -27980,7 +27967,7 @@
       <c r="L3" s="28"/>
       <c r="M3" s="28"/>
       <c r="N3" s="28" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="O3" s="28"/>
       <c r="P3" s="28"/>
@@ -27992,7 +27979,7 @@
       <c r="U3" s="28"/>
       <c r="V3" s="28"/>
       <c r="W3" s="28" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="X3" s="28"/>
       <c r="Y3" s="28"/>
@@ -28021,7 +28008,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="J4" s="30">
         <v>1</v>
@@ -28051,7 +28038,7 @@
         <v>1</v>
       </c>
       <c r="T4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="U4" s="13">
         <v>2</v>
@@ -28063,7 +28050,7 @@
         <v>1</v>
       </c>
       <c r="X4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Y4" s="13">
         <v>13</v>
@@ -28166,10 +28153,10 @@
         <v>142</v>
       </c>
       <c r="G6" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H6" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J6" s="26">
         <v>3</v>
@@ -28190,16 +28177,16 @@
         <v>241</v>
       </c>
       <c r="P6" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S6">
         <v>3</v>
       </c>
       <c r="T6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="U6">
         <v>4</v>
@@ -28211,7 +28198,7 @@
         <v>3</v>
       </c>
       <c r="X6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Y6">
         <v>4</v>
@@ -28264,16 +28251,16 @@
         <v>242</v>
       </c>
       <c r="P7" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q7" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S7">
         <v>4</v>
       </c>
       <c r="T7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="U7">
         <v>2</v>
@@ -28285,7 +28272,7 @@
         <v>4</v>
       </c>
       <c r="X7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="Y7">
         <v>2</v>
@@ -28341,7 +28328,7 @@
         <v>5</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="S8">
         <v>5</v>
@@ -28421,7 +28408,7 @@
         <v>6</v>
       </c>
       <c r="T9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="U9">
         <v>5</v>
@@ -28433,7 +28420,7 @@
         <v>6</v>
       </c>
       <c r="X9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Y9">
         <v>5</v>
@@ -28483,13 +28470,13 @@
         <v>7</v>
       </c>
       <c r="O10" s="26" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="P10" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q10" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S10" s="26">
         <v>7</v>
@@ -28510,10 +28497,10 @@
         <v>134</v>
       </c>
       <c r="Y10" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Z10" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -28551,7 +28538,7 @@
         <v>12</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N11">
         <v>8</v>
@@ -28563,7 +28550,7 @@
         <v>12</v>
       </c>
       <c r="Q11" s="13" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="S11">
         <v>8</v>
@@ -28626,7 +28613,7 @@
         <v>12</v>
       </c>
       <c r="M12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N12">
         <v>9</v>
@@ -28644,7 +28631,7 @@
         <v>9</v>
       </c>
       <c r="T12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="U12" s="13">
         <v>13</v>
@@ -28656,7 +28643,7 @@
         <v>9</v>
       </c>
       <c r="X12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Y12" s="13">
         <v>10</v>
@@ -28736,7 +28723,7 @@
         <v>13</v>
       </c>
       <c r="Z13" s="13" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -28774,7 +28761,7 @@
         <v>12</v>
       </c>
       <c r="M14" s="13" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="N14">
         <v>11</v>
@@ -28792,7 +28779,7 @@
         <v>11</v>
       </c>
       <c r="T14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="U14" s="13">
         <v>9</v>
@@ -28804,7 +28791,7 @@
         <v>11</v>
       </c>
       <c r="X14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="Y14" s="13">
         <v>10</v>
@@ -28833,10 +28820,10 @@
         <v>134</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H15" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J15">
         <v>12</v>
@@ -28860,13 +28847,13 @@
         <v>12</v>
       </c>
       <c r="Q15" s="13" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="S15">
         <v>12</v>
       </c>
       <c r="T15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="U15">
         <v>13</v>
@@ -28878,7 +28865,7 @@
         <v>12</v>
       </c>
       <c r="X15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="Y15">
         <v>13</v>
@@ -28898,7 +28885,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E16">
         <v>13</v>
@@ -28910,7 +28897,7 @@
         <v>11</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="J16" s="3">
         <v>13</v>
@@ -28940,7 +28927,7 @@
         <v>13</v>
       </c>
       <c r="T16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="U16" s="13">
         <v>0</v>
@@ -28952,13 +28939,13 @@
         <v>13</v>
       </c>
       <c r="X16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Y16" s="13" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Z16" s="13" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -28972,7 +28959,7 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E17">
         <v>14</v>
@@ -29055,10 +29042,10 @@
         <v>151</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H18" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J18">
         <v>15</v>
@@ -29082,13 +29069,13 @@
         <v>19</v>
       </c>
       <c r="Q18" s="13" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="S18">
         <v>15</v>
       </c>
       <c r="T18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="U18">
         <v>16</v>
@@ -29100,7 +29087,7 @@
         <v>15</v>
       </c>
       <c r="X18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Y18">
         <v>16</v>
@@ -29129,10 +29116,10 @@
         <v>152</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J19">
         <v>16</v>
@@ -29162,7 +29149,7 @@
         <v>16</v>
       </c>
       <c r="T19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="U19">
         <v>14</v>
@@ -29174,7 +29161,7 @@
         <v>16</v>
       </c>
       <c r="X19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Y19">
         <v>14</v>
@@ -29203,10 +29190,10 @@
         <v>134</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H20" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J20">
         <v>17</v>
@@ -29218,7 +29205,7 @@
         <v>18</v>
       </c>
       <c r="M20" s="13" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="N20">
         <v>17</v>
@@ -29251,10 +29238,10 @@
         <v>134</v>
       </c>
       <c r="Y20" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Z20" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -29280,7 +29267,7 @@
         <v>14</v>
       </c>
       <c r="H21" s="27" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="J21">
         <v>18</v>
@@ -29304,7 +29291,7 @@
         <v>19</v>
       </c>
       <c r="Q21" s="13" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="S21">
         <v>18</v>
@@ -29351,10 +29338,10 @@
         <v>154</v>
       </c>
       <c r="G22" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H22" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J22">
         <v>19</v>
@@ -29378,7 +29365,7 @@
         <v>14</v>
       </c>
       <c r="Q22" s="13" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="S22">
         <v>19</v>
@@ -29425,10 +29412,10 @@
         <v>134</v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H23" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J23">
         <v>20</v>
@@ -29440,7 +29427,7 @@
         <v>14</v>
       </c>
       <c r="M23" s="13" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="N23">
         <v>20</v>
@@ -29458,7 +29445,7 @@
         <v>20</v>
       </c>
       <c r="T23" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="U23">
         <v>18</v>
@@ -29470,7 +29457,7 @@
         <v>20</v>
       </c>
       <c r="X23" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Y23">
         <v>18</v>
@@ -29523,10 +29510,10 @@
         <v>134</v>
       </c>
       <c r="P24" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q24" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S24">
         <v>21</v>
@@ -29573,10 +29560,10 @@
         <v>151</v>
       </c>
       <c r="G25" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H25" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J25">
         <v>22</v>
@@ -29600,13 +29587,13 @@
         <v>20</v>
       </c>
       <c r="Q25" s="13" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="S25">
         <v>22</v>
       </c>
       <c r="T25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="U25" s="6">
         <v>24</v>
@@ -29618,7 +29605,7 @@
         <v>22</v>
       </c>
       <c r="X25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Y25" s="6">
         <v>21</v>
@@ -29647,10 +29634,10 @@
         <v>156</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H26" s="27" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J26">
         <v>23</v>
@@ -29692,13 +29679,13 @@
         <v>23</v>
       </c>
       <c r="X26" s="26" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="Y26" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Z26" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -29721,10 +29708,10 @@
         <v>134</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H27" s="27" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J27" s="26">
         <v>24</v>
@@ -29745,16 +29732,16 @@
         <v>134</v>
       </c>
       <c r="P27" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q27" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S27">
         <v>24</v>
       </c>
       <c r="T27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="U27" s="6">
         <v>21</v>
@@ -29766,7 +29753,7 @@
         <v>24</v>
       </c>
       <c r="X27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Y27" s="6">
         <v>30</v>
@@ -29795,10 +29782,10 @@
         <v>157</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H28" s="27" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J28">
         <v>25</v>
@@ -29822,7 +29809,7 @@
         <v>32</v>
       </c>
       <c r="Q28" s="13" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="S28" s="26">
         <v>25</v>
@@ -29843,10 +29830,10 @@
         <v>134</v>
       </c>
       <c r="Y28" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Z28" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -29869,10 +29856,10 @@
         <v>154</v>
       </c>
       <c r="G29" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H29" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J29">
         <v>26</v>
@@ -29920,7 +29907,7 @@
         <v>30</v>
       </c>
       <c r="Z29" s="6" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -29943,10 +29930,10 @@
         <v>134</v>
       </c>
       <c r="G30" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H30" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J30">
         <v>27</v>
@@ -29976,7 +29963,7 @@
         <v>27</v>
       </c>
       <c r="T30" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="U30" s="6">
         <v>28</v>
@@ -29988,13 +29975,13 @@
         <v>27</v>
       </c>
       <c r="X30" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Y30" s="6">
         <v>30</v>
       </c>
       <c r="Z30" s="13" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -30091,10 +30078,10 @@
         <v>159</v>
       </c>
       <c r="G32" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H32" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J32">
         <v>29</v>
@@ -30139,10 +30126,10 @@
         <v>118</v>
       </c>
       <c r="Y32" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Z32" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -30165,10 +30152,10 @@
         <v>151</v>
       </c>
       <c r="G33" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H33" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J33">
         <v>30</v>
@@ -30198,7 +30185,7 @@
         <v>30</v>
       </c>
       <c r="T33" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="U33" s="6">
         <v>28</v>
@@ -30210,13 +30197,13 @@
         <v>30</v>
       </c>
       <c r="X33" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Y33" s="6">
         <v>22</v>
       </c>
       <c r="Z33" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -30239,10 +30226,10 @@
         <v>160</v>
       </c>
       <c r="G34" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H34" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J34">
         <v>31</v>
@@ -30272,7 +30259,7 @@
         <v>31</v>
       </c>
       <c r="T34" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="U34">
         <v>30</v>
@@ -30284,7 +30271,7 @@
         <v>31</v>
       </c>
       <c r="X34" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Y34">
         <v>30</v>
@@ -30313,10 +30300,10 @@
         <v>134</v>
       </c>
       <c r="G35" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H35" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J35">
         <v>32</v>
@@ -30361,10 +30348,10 @@
         <v>118</v>
       </c>
       <c r="Y35" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Z35" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -30390,7 +30377,7 @@
         <v>29</v>
       </c>
       <c r="H36" s="26" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="J36">
         <v>33</v>
@@ -30420,7 +30407,7 @@
         <v>33</v>
       </c>
       <c r="T36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="U36" s="6">
         <v>30</v>
@@ -30432,7 +30419,7 @@
         <v>33</v>
       </c>
       <c r="X36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Y36" s="6">
         <v>34</v>
@@ -30512,7 +30499,7 @@
         <v>30</v>
       </c>
       <c r="Z37" s="6" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -30535,10 +30522,10 @@
         <v>154</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H38" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J38" s="26">
         <v>35</v>
@@ -30559,16 +30546,16 @@
         <v>79</v>
       </c>
       <c r="P38" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q38" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S38">
         <v>35</v>
       </c>
       <c r="T38" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="U38" s="13">
         <v>33</v>
@@ -30580,7 +30567,7 @@
         <v>35</v>
       </c>
       <c r="X38" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="Y38" s="13">
         <v>34</v>
@@ -30609,16 +30596,16 @@
         <v>134</v>
       </c>
       <c r="G39" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H39" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S39">
         <v>36</v>
       </c>
       <c r="T39" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="U39">
         <v>37</v>
@@ -30630,7 +30617,7 @@
         <v>36</v>
       </c>
       <c r="X39" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Y39">
         <v>37</v>
@@ -30659,16 +30646,16 @@
         <v>128</v>
       </c>
       <c r="G40" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H40" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S40">
         <v>37</v>
       </c>
       <c r="T40" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="U40" s="6">
         <v>33</v>
@@ -30680,7 +30667,7 @@
         <v>37</v>
       </c>
       <c r="X40" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Y40" s="6">
         <v>35</v>
@@ -30715,7 +30702,7 @@
         <v>30</v>
       </c>
       <c r="J41" s="28" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="K41" s="28"/>
       <c r="L41" s="28"/>
@@ -30743,10 +30730,10 @@
         <v>79</v>
       </c>
       <c r="Y41" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Z41" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -30781,7 +30768,7 @@
       <c r="L42" s="28"/>
       <c r="M42" s="28"/>
       <c r="N42" s="28" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="O42" s="28"/>
       <c r="P42" s="28"/>
@@ -30804,13 +30791,13 @@
         <v>40</v>
       </c>
       <c r="F43" s="26" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="G43" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H43" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J43">
         <v>1</v>
@@ -30860,7 +30847,7 @@
         <v>41</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="J44">
         <v>2</v>
@@ -30904,13 +30891,13 @@
         <v>42</v>
       </c>
       <c r="F45" s="26" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="G45" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H45" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J45">
         <v>3</v>
@@ -30934,7 +30921,7 @@
         <v>4</v>
       </c>
       <c r="Q45" s="13" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -30957,10 +30944,10 @@
         <v>151</v>
       </c>
       <c r="G46" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H46" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J46">
         <v>4</v>
@@ -30981,10 +30968,10 @@
         <v>266</v>
       </c>
       <c r="P46" s="13" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q46" s="13" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -31010,7 +30997,7 @@
         <v>45</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="J47" s="29">
         <v>5</v>
@@ -31031,10 +31018,10 @@
         <v>267</v>
       </c>
       <c r="P47" s="29" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q47" s="29" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -31060,7 +31047,7 @@
         <v>41</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="J48" s="29">
         <v>6</v>
@@ -31081,10 +31068,10 @@
         <v>242</v>
       </c>
       <c r="P48" s="29" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q48" s="29" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -31134,7 +31121,7 @@
         <v>10</v>
       </c>
       <c r="Q49" s="13" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
@@ -31339,10 +31326,10 @@
         <v>154</v>
       </c>
       <c r="G53" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H53" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J53">
         <v>11</v>
@@ -31482,7 +31469,7 @@
         <v>13</v>
       </c>
       <c r="Q55" s="13" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
@@ -31513,10 +31500,10 @@
         <v>79</v>
       </c>
       <c r="G56" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H56" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J56">
         <v>14</v>
@@ -31574,7 +31561,7 @@
         <v>17</v>
       </c>
       <c r="Q57" s="13" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
@@ -31655,7 +31642,7 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="28" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="B60" s="28"/>
       <c r="C60" s="28"/>
@@ -31705,7 +31692,7 @@
       <c r="C61" s="28"/>
       <c r="D61" s="28"/>
       <c r="E61" s="28" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="F61" s="28"/>
       <c r="G61" s="28"/>
@@ -31940,7 +31927,7 @@
         <v>6</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="J65">
         <v>23</v>
@@ -32019,10 +32006,10 @@
         <v>79</v>
       </c>
       <c r="P66" s="29" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q66" s="29" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S66" s="3"/>
       <c r="T66" s="3"/>
@@ -32056,7 +32043,7 @@
         <v>6</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="J67">
         <v>25</v>
@@ -32080,7 +32067,7 @@
         <v>4</v>
       </c>
       <c r="Q67" s="13" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="S67" s="3"/>
       <c r="T67" s="3"/>
@@ -32254,7 +32241,7 @@
         <v>4</v>
       </c>
       <c r="Q70" s="6" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="S70" s="3"/>
       <c r="T70" s="3"/>
@@ -32599,10 +32586,10 @@
         <v>79</v>
       </c>
       <c r="P76" s="29" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q76" s="29" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S76" s="3"/>
       <c r="T76" s="3"/>
@@ -32633,10 +32620,10 @@
         <v>79</v>
       </c>
       <c r="G77" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H77" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
@@ -32674,10 +32661,10 @@
         <v>186</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
@@ -32721,7 +32708,7 @@
         <v>14</v>
       </c>
       <c r="J79" s="28" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="K79" s="28"/>
       <c r="L79" s="28"/>
@@ -32771,7 +32758,7 @@
       <c r="L80" s="28"/>
       <c r="M80" s="28"/>
       <c r="N80" s="28" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="O80" s="28"/>
       <c r="P80" s="28"/>
@@ -32829,10 +32816,10 @@
         <v>290</v>
       </c>
       <c r="P81" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q81" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S81" s="3"/>
       <c r="T81" s="3"/>
@@ -32924,7 +32911,7 @@
         <v>9</v>
       </c>
       <c r="H83" s="6" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="J83">
         <v>3</v>
@@ -33006,7 +32993,7 @@
         <v>6</v>
       </c>
       <c r="Q84" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="S84" s="3"/>
       <c r="T84" s="3"/>
@@ -33122,7 +33109,7 @@
         <v>6</v>
       </c>
       <c r="Q86" s="13" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="S86" s="3"/>
       <c r="T86" s="3"/>
@@ -33354,7 +33341,7 @@
         <v>17</v>
       </c>
       <c r="Q90" s="13" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="S90" s="3"/>
       <c r="T90" s="3"/>
@@ -33467,10 +33454,10 @@
         <v>134</v>
       </c>
       <c r="P92" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q92" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S92" s="3"/>
       <c r="T92" s="3"/>
@@ -33699,10 +33686,10 @@
         <v>134</v>
       </c>
       <c r="P96" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q96" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S96" s="3"/>
       <c r="T96" s="3"/>
@@ -33833,10 +33820,10 @@
         <v>197</v>
       </c>
       <c r="G99" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H99" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J99">
         <v>19</v>
@@ -33883,10 +33870,10 @@
         <v>151</v>
       </c>
       <c r="G100" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H100" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J100">
         <v>20</v>
@@ -33933,10 +33920,10 @@
         <v>198</v>
       </c>
       <c r="G101" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H101" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J101">
         <v>21</v>
@@ -34057,10 +34044,10 @@
         <v>307</v>
       </c>
       <c r="P103" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q103" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S103" s="3"/>
       <c r="T103" s="3"/>
@@ -34149,10 +34136,10 @@
         <v>183</v>
       </c>
       <c r="G105" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H105" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J105">
         <v>25</v>
@@ -34207,10 +34194,10 @@
         <v>200</v>
       </c>
       <c r="G106" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H106" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J106">
         <v>26</v>
@@ -34265,10 +34252,10 @@
         <v>128</v>
       </c>
       <c r="G107" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H107" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J107">
         <v>27</v>
@@ -34408,7 +34395,7 @@
         <v>29</v>
       </c>
       <c r="Q109" s="13" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="S109" s="3"/>
       <c r="T109" s="3"/>
@@ -34460,13 +34447,13 @@
         <v>30</v>
       </c>
       <c r="O110" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="P110" s="13" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q110" s="13" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S110" s="3"/>
       <c r="T110" s="3"/>
@@ -34524,7 +34511,7 @@
         <v>32</v>
       </c>
       <c r="Q111" s="6" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="S111" s="3"/>
       <c r="T111" s="3"/>
@@ -34555,10 +34542,10 @@
         <v>154</v>
       </c>
       <c r="G112" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H112" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J112">
         <v>32</v>
@@ -34582,7 +34569,7 @@
         <v>32</v>
       </c>
       <c r="Q112" s="6" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="S112" s="3"/>
       <c r="T112" s="3"/>
@@ -34613,10 +34600,10 @@
         <v>134</v>
       </c>
       <c r="G113" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H113" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J113">
         <v>33</v>
@@ -34671,10 +34658,10 @@
         <v>95</v>
       </c>
       <c r="G114" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H114" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J114">
         <v>34</v>
@@ -34729,10 +34716,10 @@
         <v>128</v>
       </c>
       <c r="G115" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H115" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J115">
         <v>35</v>
@@ -34845,10 +34832,10 @@
         <v>79</v>
       </c>
       <c r="G117" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H117" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="J117">
         <v>37</v>
@@ -34953,7 +34940,7 @@
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="28" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
@@ -34981,10 +34968,10 @@
         <v>117</v>
       </c>
       <c r="P120" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q120" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S120" s="3"/>
       <c r="T120" s="3"/>
@@ -35003,7 +34990,7 @@
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
       <c r="E121" s="28" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="F121" s="28"/>
       <c r="G121" s="28"/>
@@ -35027,10 +35014,10 @@
         <v>79</v>
       </c>
       <c r="P121" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="Q121" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="S121" s="3"/>
       <c r="T121" s="3"/>
@@ -35165,10 +35152,10 @@
         <v>208</v>
       </c>
       <c r="G125" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H125" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="R125" s="3"/>
       <c r="S125" s="3"/>
@@ -35340,10 +35327,10 @@
         <v>211</v>
       </c>
       <c r="G130" s="29" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H130" s="29" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="R130" s="3"/>
       <c r="S130" s="3"/>
@@ -35378,7 +35365,7 @@
         <v>25</v>
       </c>
       <c r="H131" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="R131" s="3"/>
       <c r="S131" s="3"/>
@@ -35553,7 +35540,7 @@
         <v>16</v>
       </c>
       <c r="H136" s="6" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="R136" s="3"/>
       <c r="S136" s="3"/>
@@ -35825,7 +35812,7 @@
         <v>22</v>
       </c>
       <c r="H144" s="13" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="R144" s="3"/>
       <c r="S144" s="3"/>
@@ -35892,10 +35879,10 @@
         <v>128</v>
       </c>
       <c r="G146" s="29" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H146" s="29" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="R146" s="3"/>
       <c r="S146" s="3"/>
@@ -36210,7 +36197,7 @@
         <v>26</v>
       </c>
       <c r="H155" s="6" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="R155" s="3"/>
       <c r="S155" s="3"/>
@@ -36382,10 +36369,10 @@
         <v>79</v>
       </c>
       <c r="G160" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H160" s="26" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="R160" s="3"/>
       <c r="S160" s="3"/>

</xml_diff>